<commit_message>
Add code to Federal/Schedule8812.xlsx
</commit_message>
<xml_diff>
--- a/Federal/Schedule8812.xlsx
+++ b/Federal/Schedule8812.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Schedule8812" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Note: If you have more than four dependents identified with an ITIN and listed as a qualifying child for the child tax credit, see separate instructions and check here</t>
   </si>
@@ -356,11 +356,18 @@
       <t xml:space="preserve">Form 1040, line 67, Form 1040A, line 43, or Form 1040NR, line 64 </t>
     </r>
   </si>
+  <si>
+    <t>How many qualifying children do you have?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;???_);_(@_)"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -692,7 +699,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="60">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1207,21 +1214,6 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -1401,9 +1393,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1446,13 +1485,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1521,15 +1560,6 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1599,50 +1629,41 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="53" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="52" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="55" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1650,9 +1671,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1661,50 +1679,111 @@
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="45" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="49" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="51" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="35" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="59" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="60" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="61" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="56" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="58" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="57" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="35" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="43">
+    <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="34" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="38" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="42" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="23" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="27" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="31" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="35" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="39" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="8" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="12" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="14" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Explanatory Text" xfId="17" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="7" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="5" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="6" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="10" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="16" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="15" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1982,10 +2061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2009,115 +2088,117 @@
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="41"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="38"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="46"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="43"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="47"/>
-      <c r="B3" s="48" t="s">
+      <c r="A3" s="44"/>
+      <c r="B3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="51"/>
-      <c r="M3" s="52"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="78"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="76"/>
+      <c r="B4" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="77"/>
+      <c r="D4" s="77"/>
+      <c r="E4" s="77"/>
+      <c r="F4" s="77"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
+      <c r="I4" s="77"/>
+      <c r="J4" s="77"/>
+      <c r="K4" s="77"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="44" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="46"/>
-    </row>
-    <row r="5" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="53">
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="79"/>
+    </row>
+    <row r="6" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="4">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="4">
         <v>1</v>
       </c>
-      <c r="M5" s="54"/>
-    </row>
-    <row r="6" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="55"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="56"/>
-    </row>
-    <row r="7" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="55"/>
-      <c r="B7" s="12" t="s">
-        <v>7</v>
-      </c>
+      <c r="M6" s="67"/>
+    </row>
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
@@ -2128,11 +2209,13 @@
       <c r="J7" s="13"/>
       <c r="K7" s="14"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="56"/>
-    </row>
-    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="55"/>
-      <c r="B8" s="12"/>
+      <c r="M7" s="68"/>
+    </row>
+    <row r="8" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="12" t="s">
+        <v>7</v>
+      </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
@@ -2143,233 +2226,234 @@
       <c r="J8" s="13"/>
       <c r="K8" s="14"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="56"/>
-    </row>
-    <row r="9" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="55"/>
-      <c r="B9" s="16" t="s">
+      <c r="M8" s="68"/>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="68"/>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="56"/>
-    </row>
-    <row r="10" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="55"/>
-      <c r="B10" s="20" t="s">
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="68"/>
+    </row>
+    <row r="11" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="56"/>
-    </row>
-    <row r="11" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="55"/>
-      <c r="B11" s="16" t="s">
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="68"/>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="56"/>
-    </row>
-    <row r="12" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="55"/>
-      <c r="B12" s="20" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="68"/>
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="56"/>
-    </row>
-    <row r="13" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="55"/>
-      <c r="B13" s="16" t="s">
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="68"/>
+    </row>
+    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="56"/>
-    </row>
-    <row r="14" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="55"/>
-      <c r="B14" s="20" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="68"/>
+    </row>
+    <row r="15" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="56"/>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="57"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="58"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="68"/>
     </row>
     <row r="16" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="59">
+      <c r="A16" s="52"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="69"/>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="53">
         <v>2</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B17" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
-      <c r="J16" s="30"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="3">
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="2">
         <v>2</v>
       </c>
-      <c r="M16" s="60"/>
-    </row>
-    <row r="17" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="59">
+      <c r="M17" s="70"/>
+    </row>
+    <row r="18" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="53">
         <v>3</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B18" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
-      <c r="K17" s="34"/>
-      <c r="L17" s="3">
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="30"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="2">
         <v>3</v>
       </c>
-      <c r="M17" s="60"/>
-    </row>
-    <row r="18" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="59" t="s">
+      <c r="M18" s="70">
+        <f>M6-M17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B19" s="29" t="s">
         <v>17</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="62"/>
-    </row>
-    <row r="19" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" s="29" t="s">
-        <v>19</v>
       </c>
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="3" t="s">
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K19" s="71"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="55"/>
+    </row>
+    <row r="20" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="62"/>
-    </row>
-    <row r="20" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="53">
+      <c r="B20" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="71"/>
+      <c r="J20" s="54"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="55"/>
+    </row>
+    <row r="21" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="50">
         <v>5</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B21" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="4">
-        <v>5</v>
-      </c>
-      <c r="K20" s="26"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="62"/>
-    </row>
-    <row r="21" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="55"/>
-      <c r="B21" s="12"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -2377,135 +2461,143 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
       <c r="I21" s="14"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="62"/>
-    </row>
-    <row r="22" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="55"/>
-      <c r="B22" s="16" t="s">
+      <c r="J21" s="4">
+        <v>5</v>
+      </c>
+      <c r="K21" s="72">
+        <f>IF(K19&gt;3000,K19-3000,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="54"/>
+      <c r="M21" s="55"/>
+    </row>
+    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="51"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="54"/>
+      <c r="M22" s="55"/>
+    </row>
+    <row r="23" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="51"/>
+      <c r="B23" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="62"/>
-    </row>
-    <row r="23" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="55"/>
-      <c r="B23" s="20" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="73"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="55"/>
+    </row>
+    <row r="24" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="51"/>
+      <c r="B24" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="22"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="62"/>
-    </row>
-    <row r="24" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="55"/>
-      <c r="B24" s="16" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="55"/>
+    </row>
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="51"/>
+      <c r="B25" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="62"/>
-    </row>
-    <row r="25" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="55"/>
-      <c r="B25" s="20" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="73"/>
+      <c r="L25" s="54"/>
+      <c r="M25" s="55"/>
+    </row>
+    <row r="26" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="51"/>
+      <c r="B26" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="62"/>
-    </row>
-    <row r="26" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="57"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="6"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="62"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="54"/>
+      <c r="M26" s="55"/>
     </row>
     <row r="27" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="59">
-        <v>6</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="A27" s="52"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
       <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="25"/>
-      <c r="L27" s="3">
+      <c r="I27" s="25"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="55"/>
+    </row>
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="53">
         <v>6</v>
       </c>
-      <c r="M27" s="60"/>
-    </row>
-    <row r="28" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="63"/>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="2">
+        <v>6</v>
+      </c>
+      <c r="M28" s="75">
+        <f>K21*0.015</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="56"/>
+      <c r="B29" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="64"/>
-    </row>
-    <row r="29" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="65"/>
-      <c r="B29" s="11"/>
       <c r="C29" s="13"/>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -2516,590 +2608,622 @@
       <c r="J29" s="13"/>
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
-      <c r="M29" s="64"/>
-    </row>
-    <row r="30" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="65"/>
-      <c r="B30" s="15" t="s">
+      <c r="M29" s="57"/>
+    </row>
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="58"/>
+      <c r="B30" s="3" t="str">
+        <f>IF(M4&gt;=3,"Yes","No")</f>
+        <v>No</v>
+      </c>
+      <c r="C30" s="49"/>
+      <c r="D30" s="49"/>
+      <c r="E30" s="49"/>
+      <c r="F30" s="49"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="84"/>
+    </row>
+    <row r="31" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="58"/>
+      <c r="B31" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-      <c r="M30" s="66"/>
-    </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="65"/>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="59"/>
+    </row>
+    <row r="32" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="58"/>
+      <c r="B32" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
-      <c r="K31" s="21"/>
-      <c r="L31" s="21"/>
-      <c r="M31" s="67"/>
-    </row>
-    <row r="32" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="65"/>
-      <c r="B32" s="15" t="s">
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="60"/>
+    </row>
+    <row r="33" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="58"/>
+      <c r="B33" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-      <c r="M32" s="66"/>
-    </row>
-    <row r="33" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="65"/>
-      <c r="B33" s="19" t="s">
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="59"/>
+    </row>
+    <row r="34" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="58"/>
+      <c r="B34" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
-      <c r="J33" s="21"/>
-      <c r="K33" s="21"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="67"/>
-    </row>
-    <row r="34" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="68"/>
-      <c r="B34" s="69"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="71"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="60"/>
     </row>
     <row r="35" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="72" t="s">
+      <c r="A35" s="61"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="85" t="str">
+        <f>IF(M4&gt;=3,IF(M28&gt;=M18,"Skip part III and enter "&amp;M18&amp;" on line 13","Go to line 7"),IF(M28=0,"Stop Here.  You cannot claim this credit","Skip Part II and enter " &amp; MIN(M18,M28) &amp;" on line 13"))</f>
+        <v>Stop Here.  You cannot claim this credit</v>
+      </c>
+      <c r="D35" s="85"/>
+      <c r="E35" s="85"/>
+      <c r="F35" s="85"/>
+      <c r="G35" s="82"/>
+      <c r="H35" s="82"/>
+      <c r="I35" s="82"/>
+      <c r="J35" s="82"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="83"/>
+    </row>
+    <row r="36" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="73"/>
-      <c r="H35" s="73"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="73"/>
-      <c r="M35" s="73"/>
-    </row>
-    <row r="36" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="42" t="s">
+      <c r="B36" s="66"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="66"/>
+      <c r="G36" s="66"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="66"/>
+      <c r="J36" s="66"/>
+      <c r="K36" s="66"/>
+      <c r="L36" s="66"/>
+      <c r="M36" s="66"/>
+    </row>
+    <row r="37" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="44" t="s">
+      <c r="B37" s="40"/>
+      <c r="C37" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="46"/>
-    </row>
-    <row r="37" spans="1:13" s="1" customFormat="1" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="59">
+      <c r="D37" s="42"/>
+      <c r="E37" s="42"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="42"/>
+      <c r="L37" s="42"/>
+      <c r="M37" s="43"/>
+    </row>
+    <row r="38" spans="1:13" s="1" customFormat="1" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="53">
         <v>7</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B38" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
-      <c r="J37" s="3">
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="2">
         <v>7</v>
       </c>
-      <c r="K37" s="2"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="62"/>
-    </row>
-    <row r="38" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="53">
+      <c r="K38" s="71"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="55"/>
+    </row>
+    <row r="39" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="50">
         <v>8</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B39" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="39"/>
-      <c r="D38" s="39"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="4">
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="4">
         <v>8</v>
       </c>
-      <c r="K38" s="26"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="62"/>
-    </row>
-    <row r="39" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="55"/>
-      <c r="B39" s="20" t="s">
+      <c r="K39" s="72"/>
+      <c r="L39" s="54"/>
+      <c r="M39" s="55"/>
+    </row>
+    <row r="40" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="51"/>
+      <c r="B40" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="21"/>
-      <c r="D39" s="21"/>
-      <c r="E39" s="21"/>
-      <c r="F39" s="21"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="5"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="62"/>
-    </row>
-    <row r="40" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="55"/>
-      <c r="B40" s="16" t="s">
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="5"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="54"/>
+      <c r="M40" s="55"/>
+    </row>
+    <row r="41" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="51"/>
+      <c r="B41" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="18"/>
-      <c r="J40" s="5"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="62"/>
-    </row>
-    <row r="41" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="55"/>
-      <c r="B41" s="20" t="s">
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="18"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="54"/>
+      <c r="M41" s="55"/>
+    </row>
+    <row r="42" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="51"/>
+      <c r="B42" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="21"/>
-      <c r="D41" s="21"/>
-      <c r="E41" s="21"/>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="5"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="62"/>
-    </row>
-    <row r="42" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="55"/>
-      <c r="B42" s="16" t="s">
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="22"/>
+      <c r="J42" s="5"/>
+      <c r="K42" s="73"/>
+      <c r="L42" s="54"/>
+      <c r="M42" s="55"/>
+    </row>
+    <row r="43" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="51"/>
+      <c r="B43" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="18"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="61"/>
-      <c r="M42" s="62"/>
-    </row>
-    <row r="43" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="55"/>
-      <c r="B43" s="20" t="s">
+      <c r="C43" s="17"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="18"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="73"/>
+      <c r="L43" s="54"/>
+      <c r="M43" s="55"/>
+    </row>
+    <row r="44" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="51"/>
+      <c r="B44" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="5"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="61"/>
-      <c r="M43" s="62"/>
-    </row>
-    <row r="44" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="57"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="62"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="73"/>
+      <c r="L44" s="54"/>
+      <c r="M44" s="55"/>
     </row>
     <row r="45" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="59">
+      <c r="A45" s="52"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="54"/>
+      <c r="M45" s="55"/>
+    </row>
+    <row r="46" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="53">
         <v>9</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B46" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="30"/>
-      <c r="D45" s="30"/>
-      <c r="E45" s="30"/>
-      <c r="F45" s="30"/>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="3">
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="2">
         <v>9</v>
       </c>
-      <c r="K45" s="2"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="62"/>
-    </row>
-    <row r="46" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="53">
+      <c r="K46" s="71">
+        <f>K38+K39</f>
+        <v>0</v>
+      </c>
+      <c r="L46" s="54"/>
+      <c r="M46" s="55"/>
+    </row>
+    <row r="47" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="50">
         <v>10</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B47" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="40"/>
-      <c r="J46" s="4">
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="37"/>
+      <c r="J47" s="4">
         <v>10</v>
       </c>
-      <c r="K46" s="26"/>
-      <c r="L46" s="61"/>
-      <c r="M46" s="62"/>
-    </row>
-    <row r="47" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="55"/>
-      <c r="B47" s="20" t="s">
+      <c r="K47" s="72"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="55"/>
+    </row>
+    <row r="48" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="51"/>
+      <c r="B48" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="22"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="61"/>
-      <c r="M47" s="62"/>
-    </row>
-    <row r="48" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="55"/>
-      <c r="B48" s="16" t="s">
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="73"/>
+      <c r="L48" s="54"/>
+      <c r="M48" s="55"/>
+    </row>
+    <row r="49" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="51"/>
+      <c r="B49" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
-      <c r="E48" s="17"/>
-      <c r="F48" s="17"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="61"/>
-      <c r="M48" s="62"/>
-    </row>
-    <row r="49" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="55"/>
-      <c r="B49" s="20" t="s">
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="18"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="73"/>
+      <c r="L49" s="54"/>
+      <c r="M49" s="55"/>
+    </row>
+    <row r="50" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="51"/>
+      <c r="B50" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="22"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="61"/>
-      <c r="M49" s="62"/>
-    </row>
-    <row r="50" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="55"/>
-      <c r="B50" s="16" t="s">
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="22"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="73"/>
+      <c r="L50" s="54"/>
+      <c r="M50" s="55"/>
+    </row>
+    <row r="51" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="51"/>
+      <c r="B51" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="17"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="61"/>
-      <c r="M50" s="62"/>
-    </row>
-    <row r="51" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="55"/>
-      <c r="B51" s="20" t="s">
+      <c r="C51" s="17"/>
+      <c r="D51" s="17"/>
+      <c r="E51" s="17"/>
+      <c r="F51" s="17"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="73"/>
+      <c r="L51" s="54"/>
+      <c r="M51" s="55"/>
+    </row>
+    <row r="52" spans="1:13" s="1" customFormat="1" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="51"/>
+      <c r="B52" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C51" s="21"/>
-      <c r="D51" s="21"/>
-      <c r="E51" s="21"/>
-      <c r="F51" s="21"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="22"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="27"/>
-      <c r="L51" s="61"/>
-      <c r="M51" s="62"/>
-    </row>
-    <row r="52" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="57"/>
-      <c r="B52" s="23"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="61"/>
-      <c r="M52" s="62"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
+      <c r="E52" s="21"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="73"/>
+      <c r="L52" s="54"/>
+      <c r="M52" s="55"/>
     </row>
     <row r="53" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="59">
-        <v>11</v>
-      </c>
-      <c r="B53" s="23" t="s">
-        <v>40</v>
-      </c>
+      <c r="A53" s="52"/>
+      <c r="B53" s="23"/>
       <c r="C53" s="24"/>
       <c r="D53" s="24"/>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
       <c r="G53" s="24"/>
       <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="3">
+      <c r="I53" s="25"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="74"/>
+      <c r="L53" s="54"/>
+      <c r="M53" s="55"/>
+    </row>
+    <row r="54" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="53">
         <v>11</v>
       </c>
-      <c r="M53" s="60"/>
-    </row>
-    <row r="54" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="59">
+      <c r="B54" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" s="24"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="2">
+        <v>11</v>
+      </c>
+      <c r="M54" s="70">
+        <f>MAX(K46-K47,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="53">
         <v>12</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B55" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="30"/>
-      <c r="D54" s="30"/>
-      <c r="E54" s="30"/>
-      <c r="F54" s="30"/>
-      <c r="G54" s="30"/>
-      <c r="H54" s="30"/>
-      <c r="I54" s="30"/>
-      <c r="J54" s="30"/>
-      <c r="K54" s="31"/>
-      <c r="L54" s="3">
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="2">
         <v>12</v>
       </c>
-      <c r="M54" s="60"/>
-    </row>
-    <row r="55" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="47"/>
-      <c r="B55" s="69" t="s">
+      <c r="M55" s="70">
+        <f>MAX(M28,M54)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="44"/>
+      <c r="B56" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C55" s="70"/>
-      <c r="D55" s="70"/>
-      <c r="E55" s="70"/>
-      <c r="F55" s="70"/>
-      <c r="G55" s="70"/>
-      <c r="H55" s="70"/>
-      <c r="I55" s="70"/>
-      <c r="J55" s="70"/>
-      <c r="K55" s="70"/>
-      <c r="L55" s="70"/>
-      <c r="M55" s="71"/>
-    </row>
-    <row r="56" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="42" t="s">
+      <c r="C56" s="63"/>
+      <c r="D56" s="63"/>
+      <c r="E56" s="63"/>
+      <c r="F56" s="63"/>
+      <c r="G56" s="63"/>
+      <c r="H56" s="63"/>
+      <c r="I56" s="63"/>
+      <c r="J56" s="63"/>
+      <c r="K56" s="63"/>
+      <c r="L56" s="63"/>
+      <c r="M56" s="64"/>
+    </row>
+    <row r="57" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B56" s="43"/>
-      <c r="C56" s="44" t="s">
+      <c r="B57" s="40"/>
+      <c r="C57" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
-      <c r="H56" s="45"/>
-      <c r="I56" s="45"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="45"/>
-      <c r="L56" s="45"/>
-      <c r="M56" s="46"/>
-    </row>
-    <row r="57" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="59">
+      <c r="D57" s="42"/>
+      <c r="E57" s="42"/>
+      <c r="F57" s="42"/>
+      <c r="G57" s="42"/>
+      <c r="H57" s="42"/>
+      <c r="I57" s="42"/>
+      <c r="J57" s="42"/>
+      <c r="K57" s="42"/>
+      <c r="L57" s="42"/>
+      <c r="M57" s="43"/>
+    </row>
+    <row r="58" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="53">
         <v>13</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B58" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="36"/>
-      <c r="J57" s="36"/>
-      <c r="K57" s="37"/>
-      <c r="L57" s="3">
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="33"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="33"/>
+      <c r="H58" s="33"/>
+      <c r="I58" s="33"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="34"/>
+      <c r="L58" s="2">
         <v>13</v>
       </c>
-      <c r="M57" s="60"/>
-    </row>
-    <row r="58" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="47"/>
-      <c r="B58" s="69" t="s">
+      <c r="M58" s="86">
+        <f>MIN(M55,M18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" s="1" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="44"/>
+      <c r="B59" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="C58" s="70"/>
-      <c r="D58" s="70"/>
-      <c r="E58" s="70"/>
-      <c r="F58" s="70"/>
-      <c r="G58" s="70"/>
-      <c r="H58" s="70"/>
-      <c r="I58" s="70"/>
-      <c r="J58" s="70"/>
-      <c r="K58" s="70"/>
-      <c r="L58" s="70"/>
-      <c r="M58" s="71"/>
+      <c r="C59" s="63"/>
+      <c r="D59" s="63"/>
+      <c r="E59" s="63"/>
+      <c r="F59" s="63"/>
+      <c r="G59" s="63"/>
+      <c r="H59" s="63"/>
+      <c r="I59" s="63"/>
+      <c r="J59" s="63"/>
+      <c r="K59" s="63"/>
+      <c r="L59" s="63"/>
+      <c r="M59" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="75">
-    <mergeCell ref="B57:K57"/>
-    <mergeCell ref="B58:M58"/>
-    <mergeCell ref="A35:M35"/>
-    <mergeCell ref="J46:J52"/>
-    <mergeCell ref="K46:K52"/>
-    <mergeCell ref="B53:K53"/>
+    <mergeCell ref="B58:K58"/>
+    <mergeCell ref="B59:M59"/>
+    <mergeCell ref="A36:M36"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="J47:J53"/>
+    <mergeCell ref="K47:K53"/>
     <mergeCell ref="B54:K54"/>
-    <mergeCell ref="B55:M55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="C56:M56"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="B55:K55"/>
+    <mergeCell ref="B56:M56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="C57:M57"/>
+    <mergeCell ref="A47:A53"/>
     <mergeCell ref="B47:I47"/>
     <mergeCell ref="B48:I48"/>
     <mergeCell ref="B49:I49"/>
     <mergeCell ref="B50:I50"/>
     <mergeCell ref="B51:I51"/>
     <mergeCell ref="B52:I52"/>
-    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="B53:I53"/>
     <mergeCell ref="B43:I43"/>
     <mergeCell ref="B44:I44"/>
-    <mergeCell ref="J38:J44"/>
-    <mergeCell ref="K38:K44"/>
     <mergeCell ref="B45:I45"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:M36"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="J39:J45"/>
+    <mergeCell ref="K39:K45"/>
+    <mergeCell ref="B46:I46"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:M37"/>
     <mergeCell ref="B38:I38"/>
+    <mergeCell ref="A39:A45"/>
     <mergeCell ref="B39:I39"/>
     <mergeCell ref="B40:I40"/>
     <mergeCell ref="B41:I41"/>
-    <mergeCell ref="J20:J26"/>
-    <mergeCell ref="K20:K26"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="B28:M28"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="J21:J27"/>
+    <mergeCell ref="K21:K27"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="A29:A35"/>
     <mergeCell ref="B29:M29"/>
-    <mergeCell ref="B30:M30"/>
     <mergeCell ref="B31:M31"/>
     <mergeCell ref="B32:M32"/>
     <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="A21:A27"/>
     <mergeCell ref="B21:I21"/>
     <mergeCell ref="B22:I22"/>
     <mergeCell ref="B23:I23"/>
     <mergeCell ref="B24:I24"/>
     <mergeCell ref="B25:I25"/>
     <mergeCell ref="B26:I26"/>
-    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="B27:I27"/>
     <mergeCell ref="B15:K15"/>
-    <mergeCell ref="L5:L15"/>
-    <mergeCell ref="M5:M15"/>
     <mergeCell ref="B16:K16"/>
+    <mergeCell ref="L6:L16"/>
+    <mergeCell ref="M6:M16"/>
     <mergeCell ref="B17:K17"/>
-    <mergeCell ref="A5:A15"/>
-    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B18:K18"/>
+    <mergeCell ref="A6:A16"/>
     <mergeCell ref="B6:K6"/>
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="B8:K8"/>
@@ -3108,12 +3232,13 @@
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B12:K12"/>
     <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B14:K14"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:M2"/>
     <mergeCell ref="B3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:M4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:M5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>